<commit_message>
hypothesis testing & more graphs
</commit_message>
<xml_diff>
--- a/data/density.xlsx
+++ b/data/density.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plame\Desktop\VS Code Projects\blah\COVID-19 USA EDA\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plame\Desktop\COVID-19 in the US EDA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2C82C3-34E1-456E-88E5-9E1B7A107EA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058473E4-2CDC-4775-86F5-743EE748CF06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1343,10 +1343,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2132,6 +2132,12 @@
         <v>0.70484891252444226</v>
       </c>
     </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C52">
+        <f>_xlfn.T.TEST(C2:C45,D2:D45,2,1)</f>
+        <v>1.8140347039062036E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>